<commit_message>
Updated requirements with output example and name matching explanation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piers\automation\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piers\Git\automation_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FA2D0E-E041-4007-AA88-53B5E8EB7465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96D31445-50FC-4D66-83DC-823EDFEFCAF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-315" yWindow="705" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="2475" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>VAT Number</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>RANDSTAD PUBLIC SERVICES LIMITED</t>
+  </si>
+  <si>
+    <t>MANPOWER UK HOLDINGS LIMITED</t>
   </si>
   <si>
     <t>Valid</t>
@@ -450,12 +453,13 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -466,16 +470,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -489,7 +493,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>1</v>
@@ -547,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="b">
         <v>1</v>
@@ -587,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>0</v>
@@ -607,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="b">
         <v>0</v>
@@ -637,8 +641,24 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>

</xml_diff>